<commit_message>
debits added and funcions optmized
</commit_message>
<xml_diff>
--- a/creditos_new.xlsx
+++ b/creditos_new.xlsx
@@ -25,22 +25,22 @@
     <t>valor</t>
   </si>
   <si>
-    <t>0505</t>
-  </si>
-  <si>
-    <t>0605</t>
-  </si>
-  <si>
-    <t>0705</t>
-  </si>
-  <si>
-    <t>0805</t>
-  </si>
-  <si>
-    <t>1105</t>
-  </si>
-  <si>
-    <t>1305</t>
+    <t>05/05</t>
+  </si>
+  <si>
+    <t>05/06</t>
+  </si>
+  <si>
+    <t>05/07</t>
+  </si>
+  <si>
+    <t>05/08</t>
+  </si>
+  <si>
+    <t>05/11</t>
+  </si>
+  <si>
+    <t>05/13</t>
   </si>
   <si>
     <t xml:space="preserve">     PORTO SEGURO CIA SEG GERAIS                </t>

</xml_diff>

<commit_message>
the debt part was only working with rows with 4 words, got that fixed
</commit_message>
<xml_diff>
--- a/creditos_new.xlsx
+++ b/creditos_new.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="91">
   <si>
     <t>data</t>
   </si>
@@ -25,37 +25,82 @@
     <t>valor</t>
   </si>
   <si>
-    <t>05/05</t>
-  </si>
-  <si>
-    <t>05/06</t>
-  </si>
-  <si>
-    <t>05/07</t>
-  </si>
-  <si>
-    <t>05/08</t>
-  </si>
-  <si>
-    <t>05/11</t>
-  </si>
-  <si>
-    <t>05/13</t>
+    <t>06/01</t>
+  </si>
+  <si>
+    <t>06/02</t>
+  </si>
+  <si>
+    <t>06/03</t>
+  </si>
+  <si>
+    <t>06/04</t>
+  </si>
+  <si>
+    <t>06/05</t>
+  </si>
+  <si>
+    <t>06/08</t>
+  </si>
+  <si>
+    <t>06/09</t>
+  </si>
+  <si>
+    <t>06/10</t>
+  </si>
+  <si>
+    <t>06/12</t>
+  </si>
+  <si>
+    <t>06/15</t>
+  </si>
+  <si>
+    <t>06/16</t>
+  </si>
+  <si>
+    <t>06/17</t>
+  </si>
+  <si>
+    <t>06/18</t>
+  </si>
+  <si>
+    <t>06/19</t>
+  </si>
+  <si>
+    <t>06/22</t>
+  </si>
+  <si>
+    <t>06/23</t>
+  </si>
+  <si>
+    <t>06/24</t>
+  </si>
+  <si>
+    <t>06/25</t>
+  </si>
+  <si>
+    <t>06/26</t>
+  </si>
+  <si>
+    <t>06/29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     SUL AMERICA SEGUROS DE PESSOAS E PREVIDE   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     LIBERTY SEGUROS S.A.                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     BRADESCO AUTO RE CIA    SEGUROS            </t>
   </si>
   <si>
     <t xml:space="preserve">     PORTO SEGURO CIA SEG GERAIS                </t>
   </si>
   <si>
-    <t xml:space="preserve">     BRADESCO AUTO RE CIA    SEGUROS            </t>
-  </si>
-  <si>
     <t xml:space="preserve">     AZUL COMPANHIA DE SEGUROS GERAIS           </t>
   </si>
   <si>
-    <t xml:space="preserve">     SUL AMERICA PARTICIPACOES E INVESTIMENTO   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     LIBERTY SEGUROS S.A.                       </t>
+    <t xml:space="preserve">     SUL AMERICA SEGUROS DE AUTOMOVEIS E MASS   </t>
   </si>
   <si>
     <t xml:space="preserve">     SUHAI SEGURADORA S A                       </t>
@@ -64,52 +109,184 @@
     <t xml:space="preserve">     MAPFRE SEGUROS GERAIS S.A.                 </t>
   </si>
   <si>
-    <t xml:space="preserve">     SUL AMERICA SEGUROS DE AUTOMOVEIS E MASS   </t>
-  </si>
-  <si>
-    <t>102.44</t>
-  </si>
-  <si>
-    <t>476.96</t>
-  </si>
-  <si>
-    <t>989.72</t>
-  </si>
-  <si>
-    <t>1.197.08</t>
-  </si>
-  <si>
-    <t>263.36</t>
-  </si>
-  <si>
-    <t>55.46</t>
-  </si>
-  <si>
-    <t>171.19</t>
-  </si>
-  <si>
-    <t>654.19</t>
-  </si>
-  <si>
-    <t>185.01</t>
-  </si>
-  <si>
-    <t>149.62</t>
-  </si>
-  <si>
-    <t>1.690.84</t>
-  </si>
-  <si>
-    <t>128.01</t>
-  </si>
-  <si>
-    <t>892.07</t>
-  </si>
-  <si>
-    <t>326.34</t>
-  </si>
-  <si>
-    <t>448.92</t>
+    <t xml:space="preserve">     TOKIO MARINE SEGURADORA S A                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     HDI SEGUROS S A                            </t>
+  </si>
+  <si>
+    <t>39,00</t>
+  </si>
+  <si>
+    <t>146,30</t>
+  </si>
+  <si>
+    <t>223,44</t>
+  </si>
+  <si>
+    <t>73,65</t>
+  </si>
+  <si>
+    <t>234,16</t>
+  </si>
+  <si>
+    <t>1.385,43</t>
+  </si>
+  <si>
+    <t>463,91</t>
+  </si>
+  <si>
+    <t>66,15</t>
+  </si>
+  <si>
+    <t>188,35</t>
+  </si>
+  <si>
+    <t>906,86</t>
+  </si>
+  <si>
+    <t>916,16</t>
+  </si>
+  <si>
+    <t>381,76</t>
+  </si>
+  <si>
+    <t>169,87</t>
+  </si>
+  <si>
+    <t>75,33</t>
+  </si>
+  <si>
+    <t>81,31</t>
+  </si>
+  <si>
+    <t>114,79</t>
+  </si>
+  <si>
+    <t>369,11</t>
+  </si>
+  <si>
+    <t>281,82</t>
+  </si>
+  <si>
+    <t>196,72</t>
+  </si>
+  <si>
+    <t>210,55</t>
+  </si>
+  <si>
+    <t>216,77</t>
+  </si>
+  <si>
+    <t>205,01</t>
+  </si>
+  <si>
+    <t>780,35</t>
+  </si>
+  <si>
+    <t>306,06</t>
+  </si>
+  <si>
+    <t>324,11</t>
+  </si>
+  <si>
+    <t>750,13</t>
+  </si>
+  <si>
+    <t>540,39</t>
+  </si>
+  <si>
+    <t>280,40</t>
+  </si>
+  <si>
+    <t>332,45</t>
+  </si>
+  <si>
+    <t>155,90</t>
+  </si>
+  <si>
+    <t>147,01</t>
+  </si>
+  <si>
+    <t>150,41</t>
+  </si>
+  <si>
+    <t>259,54</t>
+  </si>
+  <si>
+    <t>336,04</t>
+  </si>
+  <si>
+    <t>266,42</t>
+  </si>
+  <si>
+    <t>1.462,18</t>
+  </si>
+  <si>
+    <t>284,91</t>
+  </si>
+  <si>
+    <t>775,45</t>
+  </si>
+  <si>
+    <t>120,67</t>
+  </si>
+  <si>
+    <t>111,66</t>
+  </si>
+  <si>
+    <t>100,67</t>
+  </si>
+  <si>
+    <t>1.100,95</t>
+  </si>
+  <si>
+    <t>189,54</t>
+  </si>
+  <si>
+    <t>384,74</t>
+  </si>
+  <si>
+    <t>139,68</t>
+  </si>
+  <si>
+    <t>1.074,58</t>
+  </si>
+  <si>
+    <t>1.206,14</t>
+  </si>
+  <si>
+    <t>403,26</t>
+  </si>
+  <si>
+    <t>145,51</t>
+  </si>
+  <si>
+    <t>1.113,49</t>
+  </si>
+  <si>
+    <t>201,37</t>
+  </si>
+  <si>
+    <t>705,45</t>
+  </si>
+  <si>
+    <t>137,97</t>
+  </si>
+  <si>
+    <t>271,48</t>
+  </si>
+  <si>
+    <t>389,80</t>
+  </si>
+  <si>
+    <t>156,08</t>
+  </si>
+  <si>
+    <t>841,48</t>
+  </si>
+  <si>
+    <t>46,71</t>
   </si>
 </sst>
 </file>
@@ -467,7 +644,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -489,10 +666,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -500,10 +677,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -511,10 +688,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -522,10 +699,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -533,21 +710,21 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -555,10 +732,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -566,21 +743,21 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -588,43 +765,43 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -632,21 +809,494 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
         <v>11</v>
       </c>
-      <c r="C16" t="s">
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
         <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" t="s">
+        <v>26</v>
+      </c>
+      <c r="C55" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>22</v>
+      </c>
+      <c r="B56" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" t="s">
+        <v>27</v>
+      </c>
+      <c r="C58" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>22</v>
+      </c>
+      <c r="B59" t="s">
+        <v>30</v>
+      </c>
+      <c r="C59" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>